<commit_message>
Actualiza base de datos EC y agrega parte 1 de nuevos estado de cuenta
</commit_message>
<xml_diff>
--- a/Data/EC/NIT-8060123490.xlsx
+++ b/Data/EC/NIT-8060123490.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\NIYARAKY\MACROS AJUSTADAS\2- MACRO COMFENALCO CARTAGENA ACTUALIZACION\Estados De Cuenta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B18F86C2-5F0E-4280-945A-D782D541D96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{86D3E9EC-1BED-40B8-871B-121099FB8B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{25FA9FFB-64F3-4EAE-B87C-2ACABE375EC8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1796E09E-35A6-4735-8C0C-165E187AB91E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="117">
   <si>
     <t>Tipo Doc Trabajador</t>
   </si>
@@ -74,289 +74,286 @@
     <t>1708</t>
   </si>
   <si>
-    <t>1143381979</t>
-  </si>
-  <si>
-    <t>ALDAIR PINEDA MEZA</t>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>940329408121</t>
+  </si>
+  <si>
+    <t>JUAN CARLOS AIZPURUA BRACHO</t>
+  </si>
+  <si>
+    <t>1810</t>
+  </si>
+  <si>
+    <t>1811</t>
+  </si>
+  <si>
+    <t>1812</t>
+  </si>
+  <si>
+    <t>1054802863</t>
+  </si>
+  <si>
+    <t>JOSE DAVID VILLAMIL VERGARA</t>
+  </si>
+  <si>
+    <t>1901</t>
+  </si>
+  <si>
+    <t>1902</t>
+  </si>
+  <si>
+    <t>1903</t>
+  </si>
+  <si>
+    <t>1904</t>
+  </si>
+  <si>
+    <t>1905</t>
+  </si>
+  <si>
+    <t>1906</t>
+  </si>
+  <si>
+    <t>1907</t>
+  </si>
+  <si>
+    <t>1908</t>
+  </si>
+  <si>
+    <t>1909</t>
+  </si>
+  <si>
+    <t>1910</t>
+  </si>
+  <si>
+    <t>1911</t>
+  </si>
+  <si>
+    <t>1912</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2101</t>
+  </si>
+  <si>
+    <t>2102</t>
+  </si>
+  <si>
+    <t>2103</t>
+  </si>
+  <si>
+    <t>2104</t>
+  </si>
+  <si>
+    <t>2105</t>
+  </si>
+  <si>
+    <t>2106</t>
+  </si>
+  <si>
+    <t>2107</t>
+  </si>
+  <si>
+    <t>2108</t>
+  </si>
+  <si>
+    <t>2109</t>
+  </si>
+  <si>
+    <t>2110</t>
+  </si>
+  <si>
+    <t>2111</t>
+  </si>
+  <si>
+    <t>2112</t>
+  </si>
+  <si>
+    <t>1002057872</t>
+  </si>
+  <si>
+    <t>EDGAR FELIPE VERGARA CASTRO</t>
+  </si>
+  <si>
+    <t>2201</t>
+  </si>
+  <si>
+    <t>2202</t>
+  </si>
+  <si>
+    <t>2203</t>
+  </si>
+  <si>
+    <t>2204</t>
+  </si>
+  <si>
+    <t>2205</t>
+  </si>
+  <si>
+    <t>2206</t>
+  </si>
+  <si>
+    <t>2207</t>
+  </si>
+  <si>
+    <t>20374325</t>
+  </si>
+  <si>
+    <t>KARINA ESTHER MONTERROSA SEÃ?AS</t>
+  </si>
+  <si>
+    <t>1047487385</t>
+  </si>
+  <si>
+    <t>ALFONSO MARTINEZ ZAPATA</t>
+  </si>
+  <si>
+    <t>2208</t>
+  </si>
+  <si>
+    <t>2209</t>
+  </si>
+  <si>
+    <t>2210</t>
+  </si>
+  <si>
+    <t>2211</t>
+  </si>
+  <si>
+    <t>2212</t>
+  </si>
+  <si>
+    <t>2301</t>
+  </si>
+  <si>
+    <t>2302</t>
+  </si>
+  <si>
+    <t>2303</t>
+  </si>
+  <si>
+    <t>2304</t>
+  </si>
+  <si>
+    <t>2305</t>
+  </si>
+  <si>
+    <t>2306</t>
+  </si>
+  <si>
+    <t>2307</t>
+  </si>
+  <si>
+    <t>2308</t>
+  </si>
+  <si>
+    <t>2309</t>
+  </si>
+  <si>
+    <t>2310</t>
+  </si>
+  <si>
+    <t>2311</t>
+  </si>
+  <si>
+    <t>2312</t>
+  </si>
+  <si>
+    <t>2401</t>
+  </si>
+  <si>
+    <t>2402</t>
+  </si>
+  <si>
+    <t>2403</t>
+  </si>
+  <si>
+    <t>2404</t>
+  </si>
+  <si>
+    <t>2405</t>
+  </si>
+  <si>
+    <t>2406</t>
+  </si>
+  <si>
+    <t>2407</t>
+  </si>
+  <si>
+    <t>2408</t>
+  </si>
+  <si>
+    <t>2409</t>
+  </si>
+  <si>
+    <t>2410</t>
+  </si>
+  <si>
+    <t>2411</t>
+  </si>
+  <si>
+    <t>2412</t>
+  </si>
+  <si>
+    <t>2501</t>
+  </si>
+  <si>
+    <t>2502</t>
+  </si>
+  <si>
+    <t>2503</t>
+  </si>
+  <si>
+    <t>2504</t>
+  </si>
+  <si>
+    <t>2505</t>
+  </si>
+  <si>
+    <t>2506</t>
   </si>
   <si>
     <t>2507</t>
   </si>
   <si>
-    <t>2506</t>
-  </si>
-  <si>
-    <t>2505</t>
-  </si>
-  <si>
-    <t>2504</t>
-  </si>
-  <si>
-    <t>2503</t>
-  </si>
-  <si>
-    <t>2502</t>
-  </si>
-  <si>
-    <t>1047487385</t>
-  </si>
-  <si>
-    <t>ALFONSO MARTINEZ ZAPATA</t>
-  </si>
-  <si>
-    <t>2212</t>
-  </si>
-  <si>
-    <t>2211</t>
-  </si>
-  <si>
-    <t>2210</t>
-  </si>
-  <si>
-    <t>2209</t>
-  </si>
-  <si>
-    <t>2208</t>
-  </si>
-  <si>
-    <t>PE</t>
-  </si>
-  <si>
-    <t>940329408121</t>
-  </si>
-  <si>
-    <t>JUAN CARLOS AIZPURUA BRACHO</t>
-  </si>
-  <si>
-    <t>2501</t>
-  </si>
-  <si>
-    <t>2412</t>
-  </si>
-  <si>
-    <t>2411</t>
-  </si>
-  <si>
-    <t>2410</t>
-  </si>
-  <si>
-    <t>2409</t>
-  </si>
-  <si>
-    <t>2408</t>
-  </si>
-  <si>
-    <t>2407</t>
-  </si>
-  <si>
-    <t>2406</t>
-  </si>
-  <si>
-    <t>2405</t>
-  </si>
-  <si>
-    <t>2404</t>
-  </si>
-  <si>
-    <t>2403</t>
-  </si>
-  <si>
-    <t>2402</t>
-  </si>
-  <si>
-    <t>2401</t>
-  </si>
-  <si>
-    <t>2312</t>
-  </si>
-  <si>
-    <t>2311</t>
-  </si>
-  <si>
-    <t>2310</t>
-  </si>
-  <si>
-    <t>2309</t>
-  </si>
-  <si>
-    <t>2308</t>
-  </si>
-  <si>
-    <t>2307</t>
-  </si>
-  <si>
-    <t>2306</t>
-  </si>
-  <si>
-    <t>2305</t>
-  </si>
-  <si>
-    <t>2304</t>
-  </si>
-  <si>
-    <t>2303</t>
-  </si>
-  <si>
-    <t>2302</t>
-  </si>
-  <si>
-    <t>2301</t>
-  </si>
-  <si>
-    <t>2207</t>
-  </si>
-  <si>
-    <t>2206</t>
-  </si>
-  <si>
-    <t>2205</t>
-  </si>
-  <si>
-    <t>2204</t>
-  </si>
-  <si>
-    <t>2203</t>
-  </si>
-  <si>
-    <t>2202</t>
-  </si>
-  <si>
-    <t>2201</t>
-  </si>
-  <si>
-    <t>2112</t>
-  </si>
-  <si>
-    <t>2111</t>
-  </si>
-  <si>
-    <t>2110</t>
-  </si>
-  <si>
-    <t>2109</t>
-  </si>
-  <si>
-    <t>2108</t>
-  </si>
-  <si>
-    <t>2107</t>
-  </si>
-  <si>
-    <t>2106</t>
-  </si>
-  <si>
-    <t>2105</t>
-  </si>
-  <si>
-    <t>2104</t>
-  </si>
-  <si>
-    <t>2103</t>
-  </si>
-  <si>
-    <t>2102</t>
-  </si>
-  <si>
-    <t>2101</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>2010</t>
-  </si>
-  <si>
-    <t>2009</t>
-  </si>
-  <si>
-    <t>2008</t>
-  </si>
-  <si>
-    <t>2007</t>
-  </si>
-  <si>
-    <t>2006</t>
-  </si>
-  <si>
-    <t>2005</t>
-  </si>
-  <si>
-    <t>2004</t>
-  </si>
-  <si>
-    <t>2003</t>
-  </si>
-  <si>
-    <t>2002</t>
-  </si>
-  <si>
-    <t>2001</t>
-  </si>
-  <si>
-    <t>1912</t>
-  </si>
-  <si>
-    <t>1911</t>
-  </si>
-  <si>
-    <t>1910</t>
-  </si>
-  <si>
-    <t>1909</t>
-  </si>
-  <si>
-    <t>1908</t>
-  </si>
-  <si>
-    <t>1907</t>
-  </si>
-  <si>
-    <t>1906</t>
-  </si>
-  <si>
-    <t>1905</t>
-  </si>
-  <si>
-    <t>1904</t>
-  </si>
-  <si>
-    <t>1903</t>
-  </si>
-  <si>
-    <t>1902</t>
-  </si>
-  <si>
-    <t>1901</t>
-  </si>
-  <si>
-    <t>1812</t>
-  </si>
-  <si>
-    <t>1811</t>
-  </si>
-  <si>
-    <t>1810</t>
-  </si>
-  <si>
-    <t>1054802863</t>
-  </si>
-  <si>
-    <t>JOSE DAVID VILLAMIL VERGARA</t>
-  </si>
-  <si>
-    <t>1002057872</t>
-  </si>
-  <si>
-    <t>EDGAR FELIPE VERGARA CASTRO</t>
-  </si>
-  <si>
-    <t>20374325</t>
-  </si>
-  <si>
-    <t>KARINA ESTHER MONTERROSA SEÃ?AS</t>
+    <t>2508</t>
   </si>
   <si>
     <t>ESTADO DE CUENTA</t>
@@ -455,7 +452,9 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -468,9 +467,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -670,23 +667,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -714,10 +711,10 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -770,7 +767,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2377211-1D64-8B2A-FD0F-9B88C72AFB7D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52472BC8-5583-C468-FBC1-68A50C1DEB39}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1121,8 +1118,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E84B770-D5BD-4ACB-B57F-5B15CA0BF1F5}">
-  <dimension ref="B2:J173"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F936D3CB-B9CE-4026-BFA2-D37AD0CD0A87}">
+  <dimension ref="B2:J168"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:J5"/>
@@ -1146,7 +1143,7 @@
       <c r="B2" s="3"/>
       <c r="C2" s="28"/>
       <c r="D2" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
@@ -1191,7 +1188,7 @@
     <row r="6" spans="2:10" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="27"/>
@@ -1223,12 +1220,12 @@
     <row r="10" spans="2:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="27"/>
       <c r="E11" s="7">
-        <v>4926775</v>
+        <v>4646024</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -1239,17 +1236,17 @@
     <row r="12" spans="2:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F13" s="5">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -1276,13 +1273,13 @@
         <v>5</v>
       </c>
       <c r="H15" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="J15" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.35">
@@ -1310,22 +1307,22 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F17" s="18">
-        <v>52000</v>
+        <v>24999</v>
       </c>
       <c r="G17" s="18">
-        <v>1300000</v>
+        <v>781242</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
@@ -1333,22 +1330,22 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F18" s="18">
-        <v>52000</v>
+        <v>31249</v>
       </c>
       <c r="G18" s="18">
-        <v>1300000</v>
+        <v>781242</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
@@ -1356,22 +1353,22 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F19" s="18">
-        <v>52000</v>
+        <v>31249</v>
       </c>
       <c r="G19" s="18">
-        <v>1300000</v>
+        <v>781242</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
@@ -1382,19 +1379,19 @@
         <v>8</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="18">
-        <v>52000</v>
+        <v>28124</v>
       </c>
       <c r="G20" s="18">
-        <v>1300000</v>
+        <v>781242</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
@@ -1402,22 +1399,22 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F21" s="18">
-        <v>52000</v>
+        <v>31249</v>
       </c>
       <c r="G21" s="18">
-        <v>1300000</v>
+        <v>781242</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
@@ -1428,19 +1425,19 @@
         <v>8</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F22" s="18">
-        <v>52000</v>
+        <v>31249</v>
       </c>
       <c r="G22" s="18">
-        <v>1300000</v>
+        <v>781242</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
@@ -1448,22 +1445,22 @@
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B23" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D23" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="16" t="s">
-        <v>22</v>
-      </c>
       <c r="F23" s="18">
-        <v>40000</v>
+        <v>31249</v>
       </c>
       <c r="G23" s="18">
-        <v>1423500</v>
+        <v>781242</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
@@ -1474,19 +1471,19 @@
         <v>8</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D24" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="F24" s="18">
-        <v>40000</v>
+        <v>31249</v>
       </c>
       <c r="G24" s="18">
-        <v>1423500</v>
+        <v>781242</v>
       </c>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
@@ -1494,22 +1491,22 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B25" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F25" s="18">
-        <v>40000</v>
+        <v>31249</v>
       </c>
       <c r="G25" s="18">
-        <v>1423500</v>
+        <v>781242</v>
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
@@ -1520,19 +1517,19 @@
         <v>8</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F26" s="18">
-        <v>40000</v>
+        <v>31249</v>
       </c>
       <c r="G26" s="18">
-        <v>1423500</v>
+        <v>781242</v>
       </c>
       <c r="H26" s="19"/>
       <c r="I26" s="19"/>
@@ -1540,22 +1537,22 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F27" s="18">
-        <v>40000</v>
+        <v>31249</v>
       </c>
       <c r="G27" s="18">
-        <v>1423500</v>
+        <v>781242</v>
       </c>
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
@@ -1563,16 +1560,16 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F28" s="18">
         <v>31249</v>
@@ -1586,16 +1583,16 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B29" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F29" s="18">
         <v>31249</v>
@@ -1609,16 +1606,16 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B30" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F30" s="18">
         <v>31249</v>
@@ -1632,16 +1629,16 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B31" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F31" s="18">
         <v>31249</v>
@@ -1655,16 +1652,16 @@
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B32" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F32" s="18">
         <v>31249</v>
@@ -1678,16 +1675,16 @@
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F33" s="18">
         <v>31249</v>
@@ -1701,16 +1698,16 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B34" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F34" s="18">
         <v>31249</v>
@@ -1724,16 +1721,16 @@
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>31</v>
       </c>
       <c r="F35" s="18">
         <v>31249</v>
@@ -1747,16 +1744,16 @@
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>32</v>
       </c>
       <c r="F36" s="18">
         <v>31249</v>
@@ -1770,16 +1767,16 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C37" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="16" t="s">
         <v>28</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>33</v>
       </c>
       <c r="F37" s="18">
         <v>31249</v>
@@ -1793,16 +1790,16 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B38" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C38" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="16" t="s">
         <v>28</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="F38" s="18">
         <v>31249</v>
@@ -1816,16 +1813,16 @@
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B39" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D39" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="16" t="s">
         <v>29</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>35</v>
       </c>
       <c r="F39" s="18">
         <v>31249</v>
@@ -1839,16 +1836,16 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B40" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D40" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="16" t="s">
         <v>29</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>36</v>
       </c>
       <c r="F40" s="18">
         <v>31249</v>
@@ -1862,16 +1859,16 @@
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B41" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F41" s="18">
         <v>31249</v>
@@ -1885,16 +1882,16 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B42" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F42" s="18">
         <v>31249</v>
@@ -1908,16 +1905,16 @@
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B43" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F43" s="18">
         <v>31249</v>
@@ -1931,16 +1928,16 @@
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B44" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F44" s="18">
         <v>31249</v>
@@ -1954,16 +1951,16 @@
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B45" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F45" s="18">
         <v>31249</v>
@@ -1977,16 +1974,16 @@
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B46" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F46" s="18">
         <v>31249</v>
@@ -2000,16 +1997,16 @@
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B47" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F47" s="18">
         <v>31249</v>
@@ -2023,16 +2020,16 @@
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B48" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F48" s="18">
         <v>31249</v>
@@ -2046,16 +2043,16 @@
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B49" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F49" s="18">
         <v>31249</v>
@@ -2069,16 +2066,16 @@
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B50" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F50" s="18">
         <v>31249</v>
@@ -2092,16 +2089,16 @@
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B51" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F51" s="18">
         <v>31249</v>
@@ -2115,16 +2112,16 @@
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B52" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="F52" s="18">
         <v>31249</v>
@@ -2138,16 +2135,16 @@
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B53" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F53" s="18">
         <v>31249</v>
@@ -2161,16 +2158,16 @@
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B54" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F54" s="18">
         <v>31249</v>
@@ -2184,16 +2181,16 @@
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B55" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F55" s="18">
         <v>31249</v>
@@ -2207,16 +2204,16 @@
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B56" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="F56" s="18">
         <v>31249</v>
@@ -2230,16 +2227,16 @@
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B57" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F57" s="18">
         <v>31249</v>
@@ -2253,16 +2250,16 @@
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B58" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F58" s="18">
         <v>31249</v>
@@ -2276,16 +2273,16 @@
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B59" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F59" s="18">
         <v>31249</v>
@@ -2299,16 +2296,16 @@
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B60" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F60" s="18">
         <v>31249</v>
@@ -2322,16 +2319,16 @@
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B61" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F61" s="18">
         <v>31249</v>
@@ -2345,16 +2342,16 @@
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B62" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F62" s="18">
         <v>31249</v>
@@ -2368,16 +2365,16 @@
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B63" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F63" s="18">
         <v>31249</v>
@@ -2391,16 +2388,16 @@
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B64" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F64" s="18">
         <v>31249</v>
@@ -2414,16 +2411,16 @@
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B65" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="F65" s="18">
         <v>31249</v>
@@ -2437,16 +2434,16 @@
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B66" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="F66" s="18">
         <v>31249</v>
@@ -2460,16 +2457,16 @@
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B67" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E67" s="16" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="F67" s="18">
         <v>31249</v>
@@ -2483,16 +2480,16 @@
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B68" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F68" s="18">
         <v>31249</v>
@@ -2506,16 +2503,16 @@
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B69" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="F69" s="18">
         <v>31249</v>
@@ -2529,16 +2526,16 @@
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B70" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="F70" s="18">
         <v>31249</v>
@@ -2552,16 +2549,16 @@
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B71" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E71" s="16" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="F71" s="18">
         <v>31249</v>
@@ -2575,16 +2572,16 @@
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B72" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D72" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="F72" s="18">
         <v>31249</v>
@@ -2598,16 +2595,16 @@
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B73" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="F73" s="18">
         <v>31249</v>
@@ -2621,16 +2618,16 @@
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B74" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E74" s="16" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="F74" s="18">
         <v>31249</v>
@@ -2644,16 +2641,16 @@
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B75" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E75" s="16" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="F75" s="18">
         <v>31249</v>
@@ -2667,16 +2664,16 @@
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B76" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D76" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E76" s="16" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F76" s="18">
         <v>31249</v>
@@ -2690,16 +2687,16 @@
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B77" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E77" s="16" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="F77" s="18">
         <v>31249</v>
@@ -2713,16 +2710,16 @@
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B78" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E78" s="16" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F78" s="18">
         <v>31249</v>
@@ -2736,16 +2733,16 @@
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B79" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E79" s="16" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="F79" s="18">
         <v>31249</v>
@@ -2759,16 +2756,16 @@
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B80" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E80" s="16" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="F80" s="18">
         <v>31249</v>
@@ -2782,16 +2779,16 @@
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B81" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E81" s="16" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="F81" s="18">
         <v>31249</v>
@@ -2805,16 +2802,16 @@
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B82" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E82" s="16" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="F82" s="18">
         <v>31249</v>
@@ -2828,16 +2825,16 @@
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B83" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D83" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E83" s="16" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="F83" s="18">
         <v>31249</v>
@@ -2851,16 +2848,16 @@
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B84" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D84" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E84" s="16" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="F84" s="18">
         <v>31249</v>
@@ -2874,16 +2871,16 @@
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B85" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E85" s="16" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="F85" s="18">
         <v>31249</v>
@@ -2897,16 +2894,16 @@
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B86" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D86" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E86" s="16" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="F86" s="18">
         <v>31249</v>
@@ -2920,16 +2917,16 @@
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B87" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E87" s="16" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="F87" s="18">
         <v>31249</v>
@@ -2943,16 +2940,16 @@
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B88" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E88" s="16" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="F88" s="18">
         <v>31249</v>
@@ -2966,16 +2963,16 @@
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B89" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C89" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D89" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E89" s="16" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="F89" s="18">
         <v>31249</v>
@@ -2989,16 +2986,16 @@
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B90" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D90" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E90" s="16" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="F90" s="18">
         <v>31249</v>
@@ -3012,16 +3009,16 @@
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B91" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C91" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D91" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E91" s="16" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="F91" s="18">
         <v>31249</v>
@@ -3035,16 +3032,16 @@
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B92" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C92" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D92" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E92" s="16" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="F92" s="18">
         <v>31249</v>
@@ -3058,22 +3055,22 @@
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B93" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C93" s="16" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D93" s="17" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="E93" s="16" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="F93" s="18">
-        <v>31249</v>
+        <v>30284</v>
       </c>
       <c r="G93" s="18">
-        <v>781242</v>
+        <v>908526</v>
       </c>
       <c r="H93" s="19"/>
       <c r="I93" s="19"/>
@@ -3081,16 +3078,16 @@
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B94" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D94" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E94" s="16" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="F94" s="18">
         <v>31249</v>
@@ -3104,16 +3101,16 @@
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B95" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C95" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D95" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E95" s="16" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="F95" s="18">
         <v>31249</v>
@@ -3127,22 +3124,22 @@
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B96" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C96" s="16" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D96" s="17" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="E96" s="16" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="F96" s="18">
-        <v>31249</v>
+        <v>36341</v>
       </c>
       <c r="G96" s="18">
-        <v>781242</v>
+        <v>908526</v>
       </c>
       <c r="H96" s="19"/>
       <c r="I96" s="19"/>
@@ -3150,16 +3147,16 @@
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B97" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C97" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D97" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E97" s="16" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="F97" s="18">
         <v>31249</v>
@@ -3173,16 +3170,16 @@
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B98" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C98" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D98" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E98" s="16" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="F98" s="18">
         <v>31249</v>
@@ -3196,22 +3193,22 @@
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B99" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C99" s="16" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D99" s="17" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="E99" s="16" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="F99" s="18">
-        <v>31249</v>
+        <v>36341</v>
       </c>
       <c r="G99" s="18">
-        <v>781242</v>
+        <v>908526</v>
       </c>
       <c r="H99" s="19"/>
       <c r="I99" s="19"/>
@@ -3219,16 +3216,16 @@
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B100" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C100" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D100" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E100" s="16" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="F100" s="18">
         <v>31249</v>
@@ -3242,16 +3239,16 @@
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B101" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C101" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D101" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E101" s="16" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="F101" s="18">
         <v>31249</v>
@@ -3265,22 +3262,22 @@
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B102" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C102" s="16" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D102" s="17" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="E102" s="16" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="F102" s="18">
-        <v>31249</v>
+        <v>36341</v>
       </c>
       <c r="G102" s="18">
-        <v>781242</v>
+        <v>908526</v>
       </c>
       <c r="H102" s="19"/>
       <c r="I102" s="19"/>
@@ -3288,16 +3285,16 @@
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B103" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C103" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D103" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E103" s="16" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="F103" s="18">
         <v>31249</v>
@@ -3311,16 +3308,16 @@
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B104" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C104" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D104" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E104" s="16" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="F104" s="18">
         <v>31249</v>
@@ -3334,22 +3331,22 @@
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B105" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C105" s="16" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D105" s="17" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="E105" s="16" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="F105" s="18">
-        <v>31249</v>
+        <v>36341</v>
       </c>
       <c r="G105" s="18">
-        <v>781242</v>
+        <v>908526</v>
       </c>
       <c r="H105" s="19"/>
       <c r="I105" s="19"/>
@@ -3357,16 +3354,16 @@
     </row>
     <row r="106" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B106" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C106" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D106" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E106" s="16" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="F106" s="18">
         <v>31249</v>
@@ -3380,16 +3377,16 @@
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B107" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C107" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D107" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E107" s="16" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="F107" s="18">
         <v>31249</v>
@@ -3403,22 +3400,22 @@
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B108" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C108" s="16" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D108" s="17" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="F108" s="18">
-        <v>31249</v>
+        <v>36341</v>
       </c>
       <c r="G108" s="18">
-        <v>781242</v>
+        <v>908526</v>
       </c>
       <c r="H108" s="19"/>
       <c r="I108" s="19"/>
@@ -3426,19 +3423,19 @@
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B109" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C109" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D109" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="F109" s="18">
-        <v>24999</v>
+        <v>31249</v>
       </c>
       <c r="G109" s="18">
         <v>781242</v>
@@ -3452,13 +3449,13 @@
         <v>8</v>
       </c>
       <c r="C110" s="16" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="D110" s="17" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="E110" s="16" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F110" s="18">
         <v>31249</v>
@@ -3475,19 +3472,19 @@
         <v>8</v>
       </c>
       <c r="C111" s="16" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
       <c r="D111" s="17" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="E111" s="16" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="F111" s="18">
-        <v>31249</v>
+        <v>36341</v>
       </c>
       <c r="G111" s="18">
-        <v>781242</v>
+        <v>908526</v>
       </c>
       <c r="H111" s="19"/>
       <c r="I111" s="19"/>
@@ -3495,16 +3492,16 @@
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B112" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C112" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D112" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E112" s="16" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="F112" s="18">
         <v>31249</v>
@@ -3521,13 +3518,13 @@
         <v>8</v>
       </c>
       <c r="C113" s="16" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="D113" s="17" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="E113" s="16" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="F113" s="18">
         <v>31249</v>
@@ -3544,19 +3541,19 @@
         <v>8</v>
       </c>
       <c r="C114" s="16" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="D114" s="17" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="E114" s="16" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="F114" s="18">
-        <v>31249</v>
+        <v>48000</v>
       </c>
       <c r="G114" s="18">
-        <v>781242</v>
+        <v>2000000</v>
       </c>
       <c r="H114" s="19"/>
       <c r="I114" s="19"/>
@@ -3567,19 +3564,19 @@
         <v>8</v>
       </c>
       <c r="C115" s="16" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="D115" s="17" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="E115" s="16" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="F115" s="18">
-        <v>31249</v>
+        <v>40000</v>
       </c>
       <c r="G115" s="18">
-        <v>781242</v>
+        <v>1000000</v>
       </c>
       <c r="H115" s="19"/>
       <c r="I115" s="19"/>
@@ -3587,16 +3584,16 @@
     </row>
     <row r="116" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B116" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C116" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D116" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E116" s="16" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="F116" s="18">
         <v>31249</v>
@@ -3613,13 +3610,13 @@
         <v>8</v>
       </c>
       <c r="C117" s="16" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="D117" s="17" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="E117" s="16" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="F117" s="18">
         <v>31249</v>
@@ -3636,19 +3633,19 @@
         <v>8</v>
       </c>
       <c r="C118" s="16" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="D118" s="17" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="E118" s="16" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F118" s="18">
-        <v>31249</v>
+        <v>40000</v>
       </c>
       <c r="G118" s="18">
-        <v>781242</v>
+        <v>1000000</v>
       </c>
       <c r="H118" s="19"/>
       <c r="I118" s="19"/>
@@ -3656,16 +3653,16 @@
     </row>
     <row r="119" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B119" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D119" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E119" s="16" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="F119" s="18">
         <v>31249</v>
@@ -3682,13 +3679,13 @@
         <v>8</v>
       </c>
       <c r="C120" s="16" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="D120" s="17" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="E120" s="16" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="F120" s="18">
         <v>31249</v>
@@ -3705,19 +3702,19 @@
         <v>8</v>
       </c>
       <c r="C121" s="16" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="D121" s="17" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="E121" s="16" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="F121" s="18">
-        <v>31249</v>
+        <v>40000</v>
       </c>
       <c r="G121" s="18">
-        <v>781242</v>
+        <v>1000000</v>
       </c>
       <c r="H121" s="19"/>
       <c r="I121" s="19"/>
@@ -3725,16 +3722,16 @@
     </row>
     <row r="122" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B122" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C122" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D122" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E122" s="16" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F122" s="18">
         <v>31249</v>
@@ -3751,13 +3748,13 @@
         <v>8</v>
       </c>
       <c r="C123" s="16" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="D123" s="17" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="E123" s="16" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F123" s="18">
         <v>31249</v>
@@ -3774,19 +3771,19 @@
         <v>8</v>
       </c>
       <c r="C124" s="16" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="D124" s="17" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="E124" s="16" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F124" s="18">
-        <v>31249</v>
+        <v>40000</v>
       </c>
       <c r="G124" s="18">
-        <v>781242</v>
+        <v>1000000</v>
       </c>
       <c r="H124" s="19"/>
       <c r="I124" s="19"/>
@@ -3794,16 +3791,16 @@
     </row>
     <row r="125" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B125" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C125" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D125" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E125" s="16" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F125" s="18">
         <v>31249</v>
@@ -3820,13 +3817,13 @@
         <v>8</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="D126" s="17" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="E126" s="16" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F126" s="18">
         <v>31249</v>
@@ -3843,19 +3840,19 @@
         <v>8</v>
       </c>
       <c r="C127" s="16" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="D127" s="17" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="E127" s="16" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F127" s="18">
-        <v>31249</v>
+        <v>40000</v>
       </c>
       <c r="G127" s="18">
-        <v>781242</v>
+        <v>1000000</v>
       </c>
       <c r="H127" s="19"/>
       <c r="I127" s="19"/>
@@ -3863,16 +3860,16 @@
     </row>
     <row r="128" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B128" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D128" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E128" s="16" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="F128" s="18">
         <v>31249</v>
@@ -3889,13 +3886,13 @@
         <v>8</v>
       </c>
       <c r="C129" s="16" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="D129" s="17" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="E129" s="16" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F129" s="18">
         <v>31249</v>
@@ -3909,16 +3906,16 @@
     </row>
     <row r="130" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B130" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C130" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D130" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E130" s="16" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F130" s="18">
         <v>31249</v>
@@ -3935,13 +3932,13 @@
         <v>8</v>
       </c>
       <c r="C131" s="16" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="D131" s="17" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="E131" s="16" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F131" s="18">
         <v>31249</v>
@@ -3955,16 +3952,16 @@
     </row>
     <row r="132" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B132" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C132" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D132" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E132" s="16" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F132" s="18">
         <v>31249</v>
@@ -3978,16 +3975,16 @@
     </row>
     <row r="133" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B133" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C133" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D133" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E133" s="16" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F133" s="18">
         <v>31249</v>
@@ -4001,16 +3998,16 @@
     </row>
     <row r="134" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B134" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C134" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D134" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E134" s="16" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F134" s="18">
         <v>31249</v>
@@ -4024,16 +4021,16 @@
     </row>
     <row r="135" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B135" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C135" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D135" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E135" s="16" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F135" s="18">
         <v>31249</v>
@@ -4047,16 +4044,16 @@
     </row>
     <row r="136" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B136" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C136" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D136" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E136" s="16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F136" s="18">
         <v>31249</v>
@@ -4070,16 +4067,16 @@
     </row>
     <row r="137" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B137" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C137" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D137" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E137" s="16" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F137" s="18">
         <v>31249</v>
@@ -4093,16 +4090,16 @@
     </row>
     <row r="138" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B138" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C138" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D138" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E138" s="16" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F138" s="18">
         <v>31249</v>
@@ -4116,16 +4113,16 @@
     </row>
     <row r="139" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B139" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C139" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D139" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E139" s="16" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F139" s="18">
         <v>31249</v>
@@ -4139,16 +4136,16 @@
     </row>
     <row r="140" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B140" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C140" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D140" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E140" s="16" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F140" s="18">
         <v>31249</v>
@@ -4162,16 +4159,16 @@
     </row>
     <row r="141" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B141" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C141" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D141" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E141" s="16" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F141" s="18">
         <v>31249</v>
@@ -4185,16 +4182,16 @@
     </row>
     <row r="142" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B142" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C142" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D142" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E142" s="16" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F142" s="18">
         <v>31249</v>
@@ -4208,16 +4205,16 @@
     </row>
     <row r="143" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B143" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C143" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D143" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E143" s="16" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F143" s="18">
         <v>31249</v>
@@ -4231,16 +4228,16 @@
     </row>
     <row r="144" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B144" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C144" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D144" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E144" s="16" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F144" s="18">
         <v>31249</v>
@@ -4254,16 +4251,16 @@
     </row>
     <row r="145" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B145" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C145" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D145" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E145" s="16" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F145" s="18">
         <v>31249</v>
@@ -4277,16 +4274,16 @@
     </row>
     <row r="146" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B146" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C146" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D146" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E146" s="16" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F146" s="18">
         <v>31249</v>
@@ -4300,16 +4297,16 @@
     </row>
     <row r="147" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B147" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C147" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D147" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E147" s="16" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F147" s="18">
         <v>31249</v>
@@ -4323,16 +4320,16 @@
     </row>
     <row r="148" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B148" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C148" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D148" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E148" s="16" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F148" s="18">
         <v>31249</v>
@@ -4346,16 +4343,16 @@
     </row>
     <row r="149" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B149" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C149" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D149" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E149" s="16" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F149" s="18">
         <v>31249</v>
@@ -4369,16 +4366,16 @@
     </row>
     <row r="150" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B150" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C150" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D150" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E150" s="16" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F150" s="18">
         <v>31249</v>
@@ -4392,16 +4389,16 @@
     </row>
     <row r="151" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B151" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C151" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D151" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E151" s="16" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F151" s="18">
         <v>31249</v>
@@ -4415,16 +4412,16 @@
     </row>
     <row r="152" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B152" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C152" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D152" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E152" s="16" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F152" s="18">
         <v>31249</v>
@@ -4438,16 +4435,16 @@
     </row>
     <row r="153" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B153" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C153" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D153" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E153" s="16" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F153" s="18">
         <v>31249</v>
@@ -4461,16 +4458,16 @@
     </row>
     <row r="154" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B154" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C154" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D154" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E154" s="16" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F154" s="18">
         <v>31249</v>
@@ -4484,16 +4481,16 @@
     </row>
     <row r="155" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B155" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C155" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D155" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E155" s="16" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F155" s="18">
         <v>31249</v>
@@ -4507,16 +4504,16 @@
     </row>
     <row r="156" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B156" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C156" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D156" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E156" s="16" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F156" s="18">
         <v>31249</v>
@@ -4530,16 +4527,16 @@
     </row>
     <row r="157" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B157" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C157" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D157" s="17" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E157" s="16" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F157" s="18">
         <v>31249</v>
@@ -4553,16 +4550,16 @@
     </row>
     <row r="158" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B158" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C158" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D158" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E158" s="16" t="s">
         <v>101</v>
-      </c>
-      <c r="D158" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="E158" s="16" t="s">
-        <v>97</v>
       </c>
       <c r="F158" s="18">
         <v>31249</v>
@@ -4576,19 +4573,19 @@
     </row>
     <row r="159" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B159" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C159" s="16" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D159" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E159" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E159" s="16" t="s">
-        <v>98</v>
-      </c>
       <c r="F159" s="18">
-        <v>28124</v>
+        <v>31249</v>
       </c>
       <c r="G159" s="18">
         <v>781242</v>
@@ -4599,22 +4596,22 @@
     </row>
     <row r="160" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B160" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C160" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D160" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E160" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="D160" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E160" s="16" t="s">
-        <v>56</v>
-      </c>
       <c r="F160" s="18">
-        <v>36341</v>
+        <v>31249</v>
       </c>
       <c r="G160" s="18">
-        <v>908526</v>
+        <v>781242</v>
       </c>
       <c r="H160" s="19"/>
       <c r="I160" s="19"/>
@@ -4622,193 +4619,78 @@
     </row>
     <row r="161" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B161" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C161" s="16" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="D161" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E161" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="E161" s="16" t="s">
-        <v>57</v>
-      </c>
       <c r="F161" s="18">
-        <v>36341</v>
+        <v>31249</v>
       </c>
       <c r="G161" s="18">
-        <v>908526</v>
+        <v>781242</v>
       </c>
       <c r="H161" s="19"/>
       <c r="I161" s="19"/>
       <c r="J161" s="20"/>
     </row>
     <row r="162" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B162" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C162" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D162" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E162" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F162" s="18">
-        <v>36341</v>
-      </c>
-      <c r="G162" s="18">
-        <v>908526</v>
-      </c>
-      <c r="H162" s="19"/>
-      <c r="I162" s="19"/>
-      <c r="J162" s="20"/>
-    </row>
-    <row r="163" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B163" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C163" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D163" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E163" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F163" s="18">
-        <v>36341</v>
-      </c>
-      <c r="G163" s="18">
-        <v>908526</v>
-      </c>
-      <c r="H163" s="19"/>
-      <c r="I163" s="19"/>
-      <c r="J163" s="20"/>
-    </row>
-    <row r="164" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B164" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C164" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D164" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E164" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F164" s="18">
-        <v>36341</v>
-      </c>
-      <c r="G164" s="18">
-        <v>908526</v>
-      </c>
-      <c r="H164" s="19"/>
-      <c r="I164" s="19"/>
-      <c r="J164" s="20"/>
-    </row>
-    <row r="165" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B165" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C165" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D165" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E165" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F165" s="18">
-        <v>36341</v>
-      </c>
-      <c r="G165" s="18">
-        <v>908526</v>
-      </c>
-      <c r="H165" s="19"/>
-      <c r="I165" s="19"/>
-      <c r="J165" s="20"/>
-    </row>
-    <row r="166" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B166" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C166" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D166" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E166" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F166" s="18">
-        <v>30284</v>
-      </c>
-      <c r="G166" s="18">
-        <v>908526</v>
-      </c>
-      <c r="H166" s="19"/>
-      <c r="I166" s="19"/>
-      <c r="J166" s="20"/>
+      <c r="B162" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C162" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D162" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E162" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F162" s="24">
+        <v>31249</v>
+      </c>
+      <c r="G162" s="24">
+        <v>781242</v>
+      </c>
+      <c r="H162" s="25"/>
+      <c r="I162" s="25"/>
+      <c r="J162" s="26"/>
     </row>
     <row r="167" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B167" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C167" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D167" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="E167" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F167" s="24">
-        <v>48000</v>
-      </c>
-      <c r="G167" s="24">
-        <v>2000000</v>
-      </c>
-      <c r="H167" s="25"/>
-      <c r="I167" s="25"/>
-      <c r="J167" s="26"/>
-    </row>
-    <row r="172" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B172" s="32" t="s">
+      <c r="B167" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C167" s="32"/>
+      <c r="H167" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I167" s="1"/>
+      <c r="J167" s="1"/>
+    </row>
+    <row r="168" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B168" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="C168" s="32"/>
+      <c r="H168" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C172" s="32"/>
-      <c r="H172" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I172" s="1"/>
-      <c r="J172" s="1"/>
-    </row>
-    <row r="173" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B173" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="C173" s="32"/>
-      <c r="H173" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I173" s="1"/>
-      <c r="J173" s="1"/>
+      <c r="I168" s="1"/>
+      <c r="J168" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B173:C173"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="H173:J173"/>
-    <mergeCell ref="H172:J172"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="H168:J168"/>
+    <mergeCell ref="H167:J167"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="D2:J5"/>

</xml_diff>